<commit_message>
Add View (Shop's View)
</commit_message>
<xml_diff>
--- a/DB/DB.xlsx
+++ b/DB/DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\14- Entity Framwork, MVC\MVC\01- lab\FinalProject\MVC_FinalProject\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Documents\GitHub\MVC_FinalProject\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7187A6-9111-4252-8637-CFC8A9043CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40A7EAC-B087-40B3-BB46-F5DECC43CBD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="38">
   <si>
     <t>Id</t>
   </si>
@@ -86,9 +97,6 @@
     <t>/Image/Products/1.png</t>
   </si>
   <si>
-    <t>/Image/Products/2.png</t>
-  </si>
-  <si>
     <t>SKU</t>
   </si>
   <si>
@@ -142,6 +150,12 @@
   <si>
     <t>VariationOptionsId</t>
   </si>
+  <si>
+    <t>/Image/Products/1.jpg</t>
+  </si>
+  <si>
+    <t>/Image/Products/2.jpg</t>
+  </si>
 </sst>
 </file>
 
@@ -176,12 +190,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D066CD61-E16B-462B-820A-B24DBFE17BD9}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,7 +569,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -567,13 +580,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -590,7 +603,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -601,13 +614,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -624,7 +637,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -635,13 +648,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -658,7 +671,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -669,13 +682,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -692,7 +705,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -703,13 +716,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -726,7 +739,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -737,13 +750,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -760,7 +773,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -771,13 +784,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
@@ -794,7 +807,7 @@
         <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -805,13 +818,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -828,7 +841,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -839,13 +852,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -862,7 +875,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -873,13 +886,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E21" s="1">
         <v>1</v>
@@ -896,7 +909,7 @@
         <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -907,13 +920,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -930,7 +943,7 @@
         <v>16</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -941,13 +954,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -964,7 +977,7 @@
         <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -975,13 +988,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
@@ -998,7 +1011,7 @@
         <v>16</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E28" s="1">
         <v>1</v>
@@ -1009,13 +1022,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -1032,7 +1045,7 @@
         <v>16</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -1043,13 +1056,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -1083,19 +1096,19 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1103,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1">
         <v>100</v>
@@ -1123,7 +1136,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1">
         <v>50</v>
@@ -1143,7 +1156,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1">
         <v>20</v>
@@ -1163,7 +1176,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -1183,7 +1196,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1">
         <v>200</v>
@@ -1203,7 +1216,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1">
         <v>300</v>
@@ -1223,7 +1236,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1">
         <v>10</v>
@@ -1243,7 +1256,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1">
         <v>60</v>
@@ -1263,7 +1276,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1">
         <v>100</v>
@@ -1283,7 +1296,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1">
         <v>50</v>
@@ -1303,7 +1316,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1">
         <v>20</v>
@@ -1323,7 +1336,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -1343,7 +1356,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1">
         <v>200</v>
@@ -1363,7 +1376,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1">
         <v>300</v>
@@ -1383,7 +1396,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1">
         <v>10</v>
@@ -1403,7 +1416,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="1">
         <v>60</v>
@@ -1423,7 +1436,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1">
         <v>100</v>
@@ -1443,7 +1456,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1">
         <v>50</v>
@@ -1463,7 +1476,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1">
         <v>20</v>
@@ -1483,7 +1496,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -1503,7 +1516,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1">
         <v>200</v>
@@ -1523,7 +1536,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1">
         <v>300</v>
@@ -1543,7 +1556,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1">
         <v>10</v>
@@ -1563,7 +1576,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1">
         <v>60</v>
@@ -1583,7 +1596,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1">
         <v>100</v>
@@ -1603,7 +1616,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1">
         <v>50</v>
@@ -1623,7 +1636,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="1">
         <v>20</v>
@@ -1643,7 +1656,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -1663,7 +1676,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1">
         <v>200</v>
@@ -1683,7 +1696,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="1">
         <v>300</v>
@@ -1703,7 +1716,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="1">
         <v>10</v>
@@ -1723,7 +1736,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="1">
         <v>60</v>
@@ -1743,7 +1756,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" s="1">
         <v>100</v>
@@ -1763,7 +1776,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C35" s="1">
         <v>50</v>
@@ -1783,7 +1796,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="1">
         <v>20</v>
@@ -1803,7 +1816,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
@@ -1823,7 +1836,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="1">
         <v>200</v>
@@ -1843,7 +1856,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="1">
         <v>300</v>
@@ -1863,7 +1876,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="1">
         <v>10</v>
@@ -1883,7 +1896,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C41" s="1">
         <v>60</v>
@@ -1903,7 +1916,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" s="1">
         <v>100</v>
@@ -1923,7 +1936,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" s="1">
         <v>50</v>
@@ -1943,7 +1956,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C44" s="1">
         <v>20</v>
@@ -1963,7 +1976,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" s="1">
         <v>0</v>
@@ -1983,7 +1996,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C46" s="1">
         <v>200</v>
@@ -2003,7 +2016,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C47" s="1">
         <v>300</v>
@@ -2023,7 +2036,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C48" s="1">
         <v>10</v>
@@ -2043,7 +2056,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C49" s="1">
         <v>60</v>
@@ -2063,7 +2076,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C50" s="1">
         <v>100</v>
@@ -2083,7 +2096,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C51" s="1">
         <v>50</v>
@@ -2103,7 +2116,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C52" s="1">
         <v>20</v>
@@ -2123,7 +2136,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
@@ -2143,7 +2156,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C54" s="1">
         <v>200</v>
@@ -2163,7 +2176,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C55" s="1">
         <v>300</v>
@@ -2183,7 +2196,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C56" s="1">
         <v>10</v>
@@ -2203,7 +2216,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C57" s="1">
         <v>60</v>
@@ -2223,7 +2236,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C58" s="1">
         <v>100</v>
@@ -2243,7 +2256,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C59" s="1">
         <v>50</v>
@@ -2263,7 +2276,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C60" s="1">
         <v>20</v>
@@ -2283,7 +2296,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C61" s="1">
         <v>0</v>
@@ -2303,7 +2316,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C62" s="1">
         <v>200</v>
@@ -2323,7 +2336,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C63" s="1">
         <v>300</v>
@@ -2343,7 +2356,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C64" s="1">
         <v>10</v>
@@ -2363,7 +2376,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C65" s="1">
         <v>60</v>
@@ -2383,7 +2396,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C66" s="1">
         <v>100</v>
@@ -2403,7 +2416,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C67" s="1">
         <v>50</v>
@@ -2423,7 +2436,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C68" s="1">
         <v>20</v>
@@ -2443,7 +2456,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C69" s="1">
         <v>0</v>
@@ -2463,7 +2476,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C70" s="1">
         <v>200</v>
@@ -2483,7 +2496,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C71" s="1">
         <v>300</v>
@@ -2503,7 +2516,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C72" s="1">
         <v>10</v>
@@ -2523,7 +2536,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C73" s="1">
         <v>60</v>
@@ -2543,7 +2556,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C74" s="1">
         <v>100</v>
@@ -2563,7 +2576,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C75" s="1">
         <v>50</v>
@@ -2583,7 +2596,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C76" s="1">
         <v>20</v>
@@ -2603,7 +2616,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C77" s="1">
         <v>0</v>
@@ -2623,7 +2636,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C78" s="1">
         <v>200</v>
@@ -2643,7 +2656,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C79" s="1">
         <v>300</v>
@@ -2663,7 +2676,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C80" s="1">
         <v>10</v>
@@ -2683,7 +2696,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C81" s="1">
         <v>60</v>
@@ -2703,7 +2716,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C82" s="1">
         <v>100</v>
@@ -2723,7 +2736,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C83" s="1">
         <v>50</v>
@@ -2743,7 +2756,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C84" s="1">
         <v>20</v>
@@ -2763,7 +2776,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C85" s="1">
         <v>0</v>
@@ -2783,7 +2796,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C86" s="1">
         <v>200</v>
@@ -2803,7 +2816,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C87" s="1">
         <v>300</v>
@@ -2823,7 +2836,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C88" s="1">
         <v>10</v>
@@ -2843,7 +2856,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C89" s="1">
         <v>60</v>
@@ -2863,7 +2876,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C90" s="1">
         <v>100</v>
@@ -2883,7 +2896,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C91" s="1">
         <v>50</v>
@@ -2903,7 +2916,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C92" s="1">
         <v>20</v>
@@ -2923,7 +2936,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C93" s="1">
         <v>0</v>
@@ -2943,7 +2956,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C94" s="1">
         <v>200</v>
@@ -2963,7 +2976,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C95" s="1">
         <v>300</v>
@@ -2983,7 +2996,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C96" s="1">
         <v>10</v>
@@ -3003,7 +3016,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C97" s="1">
         <v>60</v>
@@ -3023,7 +3036,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C98" s="1">
         <v>100</v>
@@ -3043,7 +3056,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C99" s="1">
         <v>50</v>
@@ -3063,7 +3076,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C100" s="1">
         <v>20</v>
@@ -3083,7 +3096,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C101" s="1">
         <v>0</v>
@@ -3103,7 +3116,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C102" s="1">
         <v>200</v>
@@ -3123,7 +3136,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C103" s="1">
         <v>300</v>
@@ -3143,7 +3156,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C104" s="1">
         <v>10</v>
@@ -3163,7 +3176,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C105" s="1">
         <v>60</v>
@@ -3183,7 +3196,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C106" s="1">
         <v>100</v>
@@ -3203,7 +3216,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C107" s="1">
         <v>50</v>
@@ -3223,7 +3236,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C108" s="1">
         <v>20</v>
@@ -3243,7 +3256,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C109" s="1">
         <v>0</v>
@@ -3263,7 +3276,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C110" s="1">
         <v>200</v>
@@ -3283,7 +3296,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C111" s="1">
         <v>300</v>
@@ -3303,7 +3316,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C112" s="1">
         <v>10</v>
@@ -3323,7 +3336,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C113" s="1">
         <v>60</v>
@@ -3343,7 +3356,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C114" s="1">
         <v>100</v>
@@ -3363,7 +3376,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C115" s="1">
         <v>50</v>
@@ -3383,7 +3396,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C116" s="1">
         <v>20</v>
@@ -3403,7 +3416,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C117" s="1">
         <v>0</v>
@@ -3423,7 +3436,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C118" s="1">
         <v>200</v>
@@ -3443,7 +3456,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C119" s="1">
         <v>300</v>
@@ -3463,7 +3476,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C120" s="1">
         <v>10</v>
@@ -3483,7 +3496,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C121" s="1">
         <v>60</v>
@@ -3589,7 +3602,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3600,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3632,9 +3645,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F1009-4870-4B7C-B1D7-976DA57B3E6B}">
-  <dimension ref="A1:G241"/>
+  <dimension ref="A1:B241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -3644,15 +3657,15 @@
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3660,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3668,7 +3681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>A2+1</f>
         <v>2</v>
@@ -3677,7 +3690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>A4</f>
         <v>2</v>
@@ -3686,7 +3699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" ref="A6" si="0">A4+1</f>
         <v>3</v>
@@ -3695,16 +3708,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" ref="A7:A70" si="1">A6</f>
+        <f t="shared" ref="A7" si="1">A6</f>
         <v>3</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" ref="A8" si="2">A6+1</f>
         <v>4</v>
@@ -3712,19 +3725,17 @@
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" ref="A9:A72" si="3">A8</f>
+        <f t="shared" ref="A9" si="3">A8</f>
         <v>4</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" ref="A10" si="4">A8+1</f>
         <v>5</v>
@@ -3732,19 +3743,17 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" ref="A11:A74" si="5">A10</f>
+        <f t="shared" ref="A11" si="5">A10</f>
         <v>5</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" ref="A12" si="6">A10+1</f>
         <v>6</v>
@@ -3752,19 +3761,17 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" ref="A13:A76" si="7">A12</f>
+        <f t="shared" ref="A13" si="7">A12</f>
         <v>6</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" ref="A14" si="8">A12+1</f>
         <v>7</v>
@@ -3772,19 +3779,17 @@
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" ref="A15:A78" si="9">A14</f>
+        <f t="shared" ref="A15" si="9">A14</f>
         <v>7</v>
       </c>
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" ref="A16" si="10">A14+1</f>
         <v>8</v>
@@ -3792,19 +3797,17 @@
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" ref="A17:A80" si="11">A16</f>
+        <f t="shared" ref="A17" si="11">A16</f>
         <v>8</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" ref="A18" si="12">A16+1</f>
         <v>9</v>
@@ -3812,19 +3815,17 @@
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" ref="A19:A82" si="13">A18</f>
+        <f t="shared" ref="A19" si="13">A18</f>
         <v>9</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" ref="A20" si="14">A18+1</f>
         <v>10</v>
@@ -3832,18 +3833,17 @@
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f t="shared" ref="A21:A84" si="15">A20</f>
+        <f t="shared" ref="A21" si="15">A20</f>
         <v>10</v>
       </c>
       <c r="B21">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" ref="A22" si="16">A20+1</f>
         <v>11</v>
@@ -3852,16 +3852,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f t="shared" ref="A23:A86" si="17">A22</f>
+        <f t="shared" ref="A23" si="17">A22</f>
         <v>11</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" ref="A24" si="18">A22+1</f>
         <v>12</v>
@@ -3870,16 +3870,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" ref="A25:A88" si="19">A24</f>
+        <f t="shared" ref="A25" si="19">A24</f>
         <v>12</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" ref="A26" si="20">A24+1</f>
         <v>13</v>
@@ -3888,16 +3888,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f t="shared" ref="A27:A90" si="21">A26</f>
+        <f t="shared" ref="A27" si="21">A26</f>
         <v>13</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" ref="A28" si="22">A26+1</f>
         <v>14</v>
@@ -3906,16 +3906,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <f t="shared" ref="A29:A92" si="23">A28</f>
+        <f t="shared" ref="A29" si="23">A28</f>
         <v>14</v>
       </c>
       <c r="B29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" ref="A30" si="24">A28+1</f>
         <v>15</v>
@@ -3924,16 +3924,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f t="shared" ref="A31:A94" si="25">A30</f>
+        <f t="shared" ref="A31" si="25">A30</f>
         <v>15</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" ref="A32" si="26">A30+1</f>
         <v>16</v>
@@ -3944,7 +3944,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <f t="shared" ref="A33:A96" si="27">A32</f>
+        <f t="shared" ref="A33" si="27">A32</f>
         <v>16</v>
       </c>
       <c r="B33">
@@ -3962,7 +3962,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <f t="shared" ref="A35:A98" si="29">A34</f>
+        <f t="shared" ref="A35" si="29">A34</f>
         <v>17</v>
       </c>
       <c r="B35">
@@ -3980,7 +3980,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <f t="shared" ref="A37:A100" si="31">A36</f>
+        <f t="shared" ref="A37" si="31">A36</f>
         <v>18</v>
       </c>
       <c r="B37">
@@ -3998,7 +3998,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <f t="shared" ref="A39:A102" si="33">A38</f>
+        <f t="shared" ref="A39" si="33">A38</f>
         <v>19</v>
       </c>
       <c r="B39">
@@ -4016,7 +4016,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <f t="shared" ref="A41:A104" si="35">A40</f>
+        <f t="shared" ref="A41" si="35">A40</f>
         <v>20</v>
       </c>
       <c r="B41">
@@ -4034,7 +4034,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <f t="shared" ref="A43:A74" si="37">A42</f>
+        <f t="shared" ref="A43" si="37">A42</f>
         <v>21</v>
       </c>
       <c r="B43">
@@ -4052,7 +4052,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <f t="shared" ref="A45:A76" si="39">A44</f>
+        <f t="shared" ref="A45" si="39">A44</f>
         <v>22</v>
       </c>
       <c r="B45">
@@ -4070,7 +4070,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <f t="shared" ref="A47:A78" si="41">A46</f>
+        <f t="shared" ref="A47" si="41">A46</f>
         <v>23</v>
       </c>
       <c r="B47">
@@ -4088,7 +4088,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <f t="shared" ref="A49:A80" si="43">A48</f>
+        <f t="shared" ref="A49" si="43">A48</f>
         <v>24</v>
       </c>
       <c r="B49">
@@ -4106,7 +4106,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
-        <f t="shared" ref="A51:A82" si="45">A50</f>
+        <f t="shared" ref="A51" si="45">A50</f>
         <v>25</v>
       </c>
       <c r="B51">
@@ -4124,7 +4124,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
-        <f t="shared" ref="A53:A84" si="47">A52</f>
+        <f t="shared" ref="A53" si="47">A52</f>
         <v>26</v>
       </c>
       <c r="B53">
@@ -4142,7 +4142,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
-        <f t="shared" ref="A55:A86" si="49">A54</f>
+        <f t="shared" ref="A55" si="49">A54</f>
         <v>27</v>
       </c>
       <c r="B55">
@@ -4160,7 +4160,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
-        <f t="shared" ref="A57:A88" si="51">A56</f>
+        <f t="shared" ref="A57" si="51">A56</f>
         <v>28</v>
       </c>
       <c r="B57">
@@ -4178,7 +4178,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
-        <f t="shared" ref="A59:A90" si="53">A58</f>
+        <f t="shared" ref="A59" si="53">A58</f>
         <v>29</v>
       </c>
       <c r="B59">
@@ -4196,7 +4196,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
-        <f t="shared" ref="A61:A92" si="55">A60</f>
+        <f t="shared" ref="A61" si="55">A60</f>
         <v>30</v>
       </c>
       <c r="B61">
@@ -4214,7 +4214,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
-        <f t="shared" ref="A63:A94" si="57">A62</f>
+        <f t="shared" ref="A63" si="57">A62</f>
         <v>31</v>
       </c>
       <c r="B63">
@@ -4232,7 +4232,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
-        <f t="shared" ref="A65:A96" si="59">A64</f>
+        <f t="shared" ref="A65" si="59">A64</f>
         <v>32</v>
       </c>
       <c r="B65">
@@ -4250,7 +4250,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
-        <f t="shared" ref="A67:A98" si="61">A66</f>
+        <f t="shared" ref="A67" si="61">A66</f>
         <v>33</v>
       </c>
       <c r="B67">
@@ -4268,7 +4268,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
-        <f t="shared" ref="A69:A100" si="63">A68</f>
+        <f t="shared" ref="A69" si="63">A68</f>
         <v>34</v>
       </c>
       <c r="B69">
@@ -4286,7 +4286,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
-        <f t="shared" ref="A71:A102" si="65">A70</f>
+        <f t="shared" ref="A71" si="65">A70</f>
         <v>35</v>
       </c>
       <c r="B71">
@@ -4304,7 +4304,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
-        <f t="shared" ref="A73:A104" si="67">A72</f>
+        <f t="shared" ref="A73" si="67">A72</f>
         <v>36</v>
       </c>
       <c r="B73">
@@ -4322,7 +4322,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
-        <f t="shared" ref="A75:A106" si="69">A74</f>
+        <f t="shared" ref="A75" si="69">A74</f>
         <v>37</v>
       </c>
       <c r="B75">
@@ -4340,7 +4340,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
-        <f t="shared" ref="A77:A108" si="71">A76</f>
+        <f t="shared" ref="A77" si="71">A76</f>
         <v>38</v>
       </c>
       <c r="B77">
@@ -4358,7 +4358,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
-        <f t="shared" ref="A79:A110" si="73">A78</f>
+        <f t="shared" ref="A79" si="73">A78</f>
         <v>39</v>
       </c>
       <c r="B79">
@@ -4376,7 +4376,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
-        <f t="shared" ref="A81:A112" si="75">A80</f>
+        <f t="shared" ref="A81" si="75">A80</f>
         <v>40</v>
       </c>
       <c r="B81">
@@ -4394,7 +4394,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
-        <f t="shared" ref="A83:A114" si="77">A82</f>
+        <f t="shared" ref="A83" si="77">A82</f>
         <v>41</v>
       </c>
       <c r="B83">
@@ -4412,7 +4412,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
-        <f t="shared" ref="A85:A116" si="79">A84</f>
+        <f t="shared" ref="A85" si="79">A84</f>
         <v>42</v>
       </c>
       <c r="B85">
@@ -4430,7 +4430,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
-        <f t="shared" ref="A87:A118" si="81">A86</f>
+        <f t="shared" ref="A87" si="81">A86</f>
         <v>43</v>
       </c>
       <c r="B87">
@@ -4448,7 +4448,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
-        <f t="shared" ref="A89:A120" si="83">A88</f>
+        <f t="shared" ref="A89" si="83">A88</f>
         <v>44</v>
       </c>
       <c r="B89">
@@ -4466,7 +4466,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
-        <f t="shared" ref="A91:A122" si="85">A90</f>
+        <f t="shared" ref="A91" si="85">A90</f>
         <v>45</v>
       </c>
       <c r="B91">
@@ -4484,7 +4484,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
-        <f t="shared" ref="A93:A124" si="87">A92</f>
+        <f t="shared" ref="A93" si="87">A92</f>
         <v>46</v>
       </c>
       <c r="B93">
@@ -4502,7 +4502,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
-        <f t="shared" ref="A95:A126" si="89">A94</f>
+        <f t="shared" ref="A95" si="89">A94</f>
         <v>47</v>
       </c>
       <c r="B95">
@@ -4520,7 +4520,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
-        <f t="shared" ref="A97:A128" si="91">A96</f>
+        <f t="shared" ref="A97" si="91">A96</f>
         <v>48</v>
       </c>
       <c r="B97">
@@ -4538,7 +4538,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
-        <f t="shared" ref="A99:A130" si="93">A98</f>
+        <f t="shared" ref="A99" si="93">A98</f>
         <v>49</v>
       </c>
       <c r="B99">
@@ -4556,7 +4556,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
-        <f t="shared" ref="A101:A132" si="95">A100</f>
+        <f t="shared" ref="A101" si="95">A100</f>
         <v>50</v>
       </c>
       <c r="B101">
@@ -4574,7 +4574,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
-        <f t="shared" ref="A103:A134" si="97">A102</f>
+        <f t="shared" ref="A103" si="97">A102</f>
         <v>51</v>
       </c>
       <c r="B103">
@@ -4592,7 +4592,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
-        <f t="shared" ref="A105:A136" si="99">A104</f>
+        <f t="shared" ref="A105" si="99">A104</f>
         <v>52</v>
       </c>
       <c r="B105">
@@ -4610,7 +4610,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
-        <f t="shared" ref="A107:A138" si="101">A106</f>
+        <f t="shared" ref="A107" si="101">A106</f>
         <v>53</v>
       </c>
       <c r="B107">
@@ -4628,7 +4628,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
-        <f t="shared" ref="A109:A140" si="103">A108</f>
+        <f t="shared" ref="A109" si="103">A108</f>
         <v>54</v>
       </c>
       <c r="B109">
@@ -4646,7 +4646,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
-        <f t="shared" ref="A111:A142" si="105">A110</f>
+        <f t="shared" ref="A111" si="105">A110</f>
         <v>55</v>
       </c>
       <c r="B111">
@@ -4664,7 +4664,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
-        <f t="shared" ref="A113:A144" si="107">A112</f>
+        <f t="shared" ref="A113" si="107">A112</f>
         <v>56</v>
       </c>
       <c r="B113">
@@ -4682,7 +4682,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
-        <f t="shared" ref="A115:A146" si="109">A114</f>
+        <f t="shared" ref="A115" si="109">A114</f>
         <v>57</v>
       </c>
       <c r="B115">
@@ -4700,7 +4700,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
-        <f t="shared" ref="A117:A148" si="111">A116</f>
+        <f t="shared" ref="A117" si="111">A116</f>
         <v>58</v>
       </c>
       <c r="B117">
@@ -4718,7 +4718,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
-        <f t="shared" ref="A119:A150" si="113">A118</f>
+        <f t="shared" ref="A119" si="113">A118</f>
         <v>59</v>
       </c>
       <c r="B119">
@@ -4736,7 +4736,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
-        <f t="shared" ref="A121:A152" si="115">A120</f>
+        <f t="shared" ref="A121" si="115">A120</f>
         <v>60</v>
       </c>
       <c r="B121">
@@ -4754,7 +4754,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
-        <f t="shared" ref="A123:A154" si="117">A122</f>
+        <f t="shared" ref="A123" si="117">A122</f>
         <v>61</v>
       </c>
       <c r="B123">
@@ -4772,7 +4772,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
-        <f t="shared" ref="A125:A156" si="119">A124</f>
+        <f t="shared" ref="A125" si="119">A124</f>
         <v>62</v>
       </c>
       <c r="B125">
@@ -4790,7 +4790,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
-        <f t="shared" ref="A127:A158" si="121">A126</f>
+        <f t="shared" ref="A127" si="121">A126</f>
         <v>63</v>
       </c>
       <c r="B127">
@@ -4808,7 +4808,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
-        <f t="shared" ref="A129:A160" si="123">A128</f>
+        <f t="shared" ref="A129" si="123">A128</f>
         <v>64</v>
       </c>
       <c r="B129">
@@ -4826,7 +4826,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
-        <f t="shared" ref="A131:A162" si="125">A130</f>
+        <f t="shared" ref="A131" si="125">A130</f>
         <v>65</v>
       </c>
       <c r="B131">
@@ -4844,7 +4844,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133">
-        <f t="shared" ref="A133:A164" si="127">A132</f>
+        <f t="shared" ref="A133" si="127">A132</f>
         <v>66</v>
       </c>
       <c r="B133">
@@ -4862,7 +4862,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135">
-        <f t="shared" ref="A135:A166" si="129">A134</f>
+        <f t="shared" ref="A135" si="129">A134</f>
         <v>67</v>
       </c>
       <c r="B135">
@@ -4880,7 +4880,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137">
-        <f t="shared" ref="A137:A168" si="131">A136</f>
+        <f t="shared" ref="A137" si="131">A136</f>
         <v>68</v>
       </c>
       <c r="B137">
@@ -4898,7 +4898,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139">
-        <f t="shared" ref="A139:A170" si="133">A138</f>
+        <f t="shared" ref="A139" si="133">A138</f>
         <v>69</v>
       </c>
       <c r="B139">
@@ -4916,7 +4916,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141">
-        <f t="shared" ref="A141:A172" si="135">A140</f>
+        <f t="shared" ref="A141" si="135">A140</f>
         <v>70</v>
       </c>
       <c r="B141">
@@ -4934,7 +4934,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143">
-        <f t="shared" ref="A143:A174" si="137">A142</f>
+        <f t="shared" ref="A143" si="137">A142</f>
         <v>71</v>
       </c>
       <c r="B143">
@@ -4952,7 +4952,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145">
-        <f t="shared" ref="A145:A176" si="139">A144</f>
+        <f t="shared" ref="A145" si="139">A144</f>
         <v>72</v>
       </c>
       <c r="B145">
@@ -4970,7 +4970,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147">
-        <f t="shared" ref="A147:A178" si="141">A146</f>
+        <f t="shared" ref="A147" si="141">A146</f>
         <v>73</v>
       </c>
       <c r="B147">
@@ -4988,7 +4988,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149">
-        <f t="shared" ref="A149:A180" si="143">A148</f>
+        <f t="shared" ref="A149" si="143">A148</f>
         <v>74</v>
       </c>
       <c r="B149">
@@ -5006,7 +5006,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151">
-        <f t="shared" ref="A151:A182" si="145">A150</f>
+        <f t="shared" ref="A151" si="145">A150</f>
         <v>75</v>
       </c>
       <c r="B151">
@@ -5024,7 +5024,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153">
-        <f t="shared" ref="A153:A184" si="147">A152</f>
+        <f t="shared" ref="A153" si="147">A152</f>
         <v>76</v>
       </c>
       <c r="B153">
@@ -5042,7 +5042,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155">
-        <f t="shared" ref="A155:A186" si="149">A154</f>
+        <f t="shared" ref="A155" si="149">A154</f>
         <v>77</v>
       </c>
       <c r="B155">
@@ -5060,7 +5060,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157">
-        <f t="shared" ref="A157:A188" si="151">A156</f>
+        <f t="shared" ref="A157" si="151">A156</f>
         <v>78</v>
       </c>
       <c r="B157">
@@ -5078,7 +5078,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159">
-        <f t="shared" ref="A159:A190" si="153">A158</f>
+        <f t="shared" ref="A159" si="153">A158</f>
         <v>79</v>
       </c>
       <c r="B159">
@@ -5096,7 +5096,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161">
-        <f t="shared" ref="A161:A192" si="155">A160</f>
+        <f t="shared" ref="A161" si="155">A160</f>
         <v>80</v>
       </c>
       <c r="B161">
@@ -5114,7 +5114,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163">
-        <f t="shared" ref="A163:A194" si="157">A162</f>
+        <f t="shared" ref="A163" si="157">A162</f>
         <v>81</v>
       </c>
       <c r="B163">
@@ -5132,7 +5132,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165">
-        <f t="shared" ref="A165:A196" si="159">A164</f>
+        <f t="shared" ref="A165" si="159">A164</f>
         <v>82</v>
       </c>
       <c r="B165">
@@ -5150,7 +5150,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167">
-        <f t="shared" ref="A167:A198" si="161">A166</f>
+        <f t="shared" ref="A167" si="161">A166</f>
         <v>83</v>
       </c>
       <c r="B167">
@@ -5168,7 +5168,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169">
-        <f t="shared" ref="A169:A200" si="163">A168</f>
+        <f t="shared" ref="A169" si="163">A168</f>
         <v>84</v>
       </c>
       <c r="B169">
@@ -5186,7 +5186,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171">
-        <f t="shared" ref="A171:A202" si="165">A170</f>
+        <f t="shared" ref="A171" si="165">A170</f>
         <v>85</v>
       </c>
       <c r="B171">
@@ -5204,7 +5204,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173">
-        <f t="shared" ref="A173:A204" si="167">A172</f>
+        <f t="shared" ref="A173" si="167">A172</f>
         <v>86</v>
       </c>
       <c r="B173">
@@ -5222,7 +5222,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175">
-        <f t="shared" ref="A175:A206" si="169">A174</f>
+        <f t="shared" ref="A175" si="169">A174</f>
         <v>87</v>
       </c>
       <c r="B175">
@@ -5240,7 +5240,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177">
-        <f t="shared" ref="A177:A208" si="171">A176</f>
+        <f t="shared" ref="A177" si="171">A176</f>
         <v>88</v>
       </c>
       <c r="B177">
@@ -5258,7 +5258,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179">
-        <f t="shared" ref="A179:A210" si="173">A178</f>
+        <f t="shared" ref="A179" si="173">A178</f>
         <v>89</v>
       </c>
       <c r="B179">
@@ -5276,7 +5276,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181">
-        <f t="shared" ref="A181:A212" si="175">A180</f>
+        <f t="shared" ref="A181" si="175">A180</f>
         <v>90</v>
       </c>
       <c r="B181">
@@ -5294,7 +5294,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183">
-        <f t="shared" ref="A183:A214" si="177">A182</f>
+        <f t="shared" ref="A183" si="177">A182</f>
         <v>91</v>
       </c>
       <c r="B183">
@@ -5312,7 +5312,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185">
-        <f t="shared" ref="A185:A216" si="179">A184</f>
+        <f t="shared" ref="A185" si="179">A184</f>
         <v>92</v>
       </c>
       <c r="B185">
@@ -5330,7 +5330,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187">
-        <f t="shared" ref="A187:A218" si="181">A186</f>
+        <f t="shared" ref="A187" si="181">A186</f>
         <v>93</v>
       </c>
       <c r="B187">
@@ -5348,7 +5348,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189">
-        <f t="shared" ref="A189:A220" si="183">A188</f>
+        <f t="shared" ref="A189" si="183">A188</f>
         <v>94</v>
       </c>
       <c r="B189">
@@ -5366,7 +5366,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191">
-        <f t="shared" ref="A191:A222" si="185">A190</f>
+        <f t="shared" ref="A191" si="185">A190</f>
         <v>95</v>
       </c>
       <c r="B191">
@@ -5384,7 +5384,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193">
-        <f t="shared" ref="A193:A224" si="187">A192</f>
+        <f t="shared" ref="A193" si="187">A192</f>
         <v>96</v>
       </c>
       <c r="B193">
@@ -5402,7 +5402,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195">
-        <f t="shared" ref="A195:A241" si="189">A194</f>
+        <f t="shared" ref="A195" si="189">A194</f>
         <v>97</v>
       </c>
       <c r="B195">
@@ -5420,7 +5420,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197">
-        <f t="shared" ref="A197:A241" si="191">A196</f>
+        <f t="shared" ref="A197" si="191">A196</f>
         <v>98</v>
       </c>
       <c r="B197">
@@ -5438,7 +5438,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199">
-        <f t="shared" ref="A199:A241" si="193">A198</f>
+        <f t="shared" ref="A199" si="193">A198</f>
         <v>99</v>
       </c>
       <c r="B199">
@@ -5456,7 +5456,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201">
-        <f t="shared" ref="A201:A241" si="195">A200</f>
+        <f t="shared" ref="A201" si="195">A200</f>
         <v>100</v>
       </c>
       <c r="B201">
@@ -5474,7 +5474,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203">
-        <f t="shared" ref="A203:A241" si="197">A202</f>
+        <f t="shared" ref="A203" si="197">A202</f>
         <v>101</v>
       </c>
       <c r="B203">
@@ -5492,7 +5492,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205">
-        <f t="shared" ref="A205:A241" si="199">A204</f>
+        <f t="shared" ref="A205" si="199">A204</f>
         <v>102</v>
       </c>
       <c r="B205">
@@ -5510,7 +5510,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207">
-        <f t="shared" ref="A207:A241" si="201">A206</f>
+        <f t="shared" ref="A207" si="201">A206</f>
         <v>103</v>
       </c>
       <c r="B207">
@@ -5528,7 +5528,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209">
-        <f t="shared" ref="A209:A241" si="203">A208</f>
+        <f t="shared" ref="A209" si="203">A208</f>
         <v>104</v>
       </c>
       <c r="B209">
@@ -5546,7 +5546,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211">
-        <f t="shared" ref="A211:A241" si="205">A210</f>
+        <f t="shared" ref="A211" si="205">A210</f>
         <v>105</v>
       </c>
       <c r="B211">
@@ -5564,7 +5564,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213">
-        <f t="shared" ref="A213:A241" si="207">A212</f>
+        <f t="shared" ref="A213" si="207">A212</f>
         <v>106</v>
       </c>
       <c r="B213">
@@ -5582,7 +5582,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215">
-        <f t="shared" ref="A215:A241" si="209">A214</f>
+        <f t="shared" ref="A215" si="209">A214</f>
         <v>107</v>
       </c>
       <c r="B215">
@@ -5600,7 +5600,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217">
-        <f t="shared" ref="A217:A241" si="211">A216</f>
+        <f t="shared" ref="A217" si="211">A216</f>
         <v>108</v>
       </c>
       <c r="B217">
@@ -5618,7 +5618,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219">
-        <f t="shared" ref="A219:A241" si="213">A218</f>
+        <f t="shared" ref="A219" si="213">A218</f>
         <v>109</v>
       </c>
       <c r="B219">
@@ -5636,7 +5636,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221">
-        <f t="shared" ref="A221:A241" si="215">A220</f>
+        <f t="shared" ref="A221" si="215">A220</f>
         <v>110</v>
       </c>
       <c r="B221">
@@ -5654,7 +5654,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223">
-        <f t="shared" ref="A223:A241" si="217">A222</f>
+        <f t="shared" ref="A223" si="217">A222</f>
         <v>111</v>
       </c>
       <c r="B223">
@@ -5672,7 +5672,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225">
-        <f t="shared" ref="A225:A241" si="219">A224</f>
+        <f t="shared" ref="A225" si="219">A224</f>
         <v>112</v>
       </c>
       <c r="B225">
@@ -5690,7 +5690,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227">
-        <f t="shared" ref="A227:A241" si="221">A226</f>
+        <f t="shared" ref="A227" si="221">A226</f>
         <v>113</v>
       </c>
       <c r="B227">
@@ -5708,7 +5708,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229">
-        <f t="shared" ref="A229:A241" si="223">A228</f>
+        <f t="shared" ref="A229" si="223">A228</f>
         <v>114</v>
       </c>
       <c r="B229">
@@ -5726,7 +5726,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231">
-        <f t="shared" ref="A231:A241" si="225">A230</f>
+        <f t="shared" ref="A231" si="225">A230</f>
         <v>115</v>
       </c>
       <c r="B231">
@@ -5744,7 +5744,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233">
-        <f t="shared" ref="A233:A241" si="227">A232</f>
+        <f t="shared" ref="A233" si="227">A232</f>
         <v>116</v>
       </c>
       <c r="B233">
@@ -5762,7 +5762,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235">
-        <f t="shared" ref="A235:A241" si="229">A234</f>
+        <f t="shared" ref="A235" si="229">A234</f>
         <v>117</v>
       </c>
       <c r="B235">
@@ -5780,7 +5780,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237">
-        <f t="shared" ref="A237:A241" si="231">A236</f>
+        <f t="shared" ref="A237" si="231">A236</f>
         <v>118</v>
       </c>
       <c r="B237">
@@ -5798,7 +5798,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239">
-        <f t="shared" ref="A239:A241" si="233">A238</f>
+        <f t="shared" ref="A239" si="233">A238</f>
         <v>119</v>
       </c>
       <c r="B239">

</xml_diff>

<commit_message>
Edit Views (Product) --and-- Seeding Stars Data
</commit_message>
<xml_diff>
--- a/DB/DB.xlsx
+++ b/DB/DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\14- Entity Framwork, MVC\MVC\01- lab\FinalProject\MVC_FinalProject\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Documents\GitHub\MVC_FinalProject\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A389D9-AF78-4263-939A-398989E8FB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C8078A-83F1-4E31-8EA0-832FE367CD96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="246">
   <si>
     <t>Id</t>
   </si>
@@ -769,6 +780,9 @@
   </si>
   <si>
     <t>BIGTREAT</t>
+  </si>
+  <si>
+    <t>Star</t>
   </si>
 </sst>
 </file>
@@ -819,17 +833,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1193,7 +1206,7 @@
       <c r="B2">
         <v>0.3</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>45992</v>
       </c>
     </row>
@@ -1204,7 +1217,7 @@
       <c r="B3">
         <v>0.15</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>45993</v>
       </c>
     </row>
@@ -1215,7 +1228,7 @@
       <c r="B4">
         <v>0.25</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>44898</v>
       </c>
     </row>
@@ -1227,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1833AB6E-1E22-4D15-9B57-21FBC3AFFCBA}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E31"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,7 +1251,7 @@
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1254,515 +1267,608 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E13" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E17" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E21" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E22" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E23" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E27" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E28" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E29" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+      <c r="E29" s="1">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E30" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E31" s="3">
-        <v>1</v>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="4">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4216,7 +4322,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76BB97CD-71B4-4425-9271-A5B35FF69E87}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -4228,7 +4334,7 @@
     <col min="3" max="3" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4239,7 +4345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4249,9 +4355,8 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4261,7 +4366,6 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>